<commit_message>
Update API Access Control Excel files
- Updated the API Access Control - Concerns and Effectiveness Excel files to incorporate the latest data and insights on API access control.
</commit_message>
<xml_diff>
--- a/data/Section 3/3.3 API Access Control/14 API Access Control- Concern.xlsx
+++ b/data/Section 3/3.3 API Access Control/14 API Access Control- Concern.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Section 3/API Access Control/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Survey Report Agent/surveyreport/data/Section 3/3.3 API Access Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{67877154-1391-404D-AAAD-02685923BEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE18C43A-C7E4-4292-A0BB-19CB3D19A16C}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{67877154-1391-404D-AAAD-02685923BEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC531196-4F03-4ADF-8110-2AEAB9AB6B80}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{96563CCE-F226-4AD8-92B2-B45C328B4391}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$J$1001</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4016" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4018" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>API access control for external users</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -238,7 +244,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,6 +259,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B67FF897-58C6-4D3A-9894-BF634A3EB748}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{B67FF897-58C6-4D3A-9894-BF634A3EB748}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6188D5FD-07D9-4A76-BF41-D29D61F037DF}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{67935AA5-C8AE-4D2C-9DD8-4A8C2303A601}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -611,10 +627,10 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -32626,10 +32642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC20222-E907-4D8F-BCE2-9C54854CBF4B}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32638,54 +32654,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>